<commit_message>
12324  1218am from PC
</commit_message>
<xml_diff>
--- a/2024/Fall 2024/TFES Lab/Heat Exchanger/HeatExchanger_DataSheet.xlsx
+++ b/2024/Fall 2024/TFES Lab/Heat Exchanger/HeatExchanger_DataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brand\Documents\SchoolFiles\2024\Fall 2024\TFES Lab\Heat Exchanger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09773130-5E13-431B-9113-E54A7CBF9145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E5686C-504E-46D2-8956-EFBA807E2997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18945" yWindow="3240" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14505" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -1516,16 +1516,19 @@
   </sheetPr>
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="8.28515625" style="32" customWidth="1"/>
-    <col min="2" max="5" width="12.85546875" style="32" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="34" customWidth="1"/>
-    <col min="7" max="9" width="12.85546875" style="32" customWidth="1"/>
+    <col min="2" max="3" width="12.85546875" style="32" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="32" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.85546875" style="32" customWidth="1"/>
     <col min="10" max="10" width="5.42578125" style="32" customWidth="1"/>
     <col min="11" max="14" width="12.85546875" style="32" customWidth="1"/>
     <col min="15" max="16384" width="8.85546875" style="32"/>

</xml_diff>